<commit_message>
Added GAP, Adjusted LULU
</commit_message>
<xml_diff>
--- a/Retail Brands/LULU_MODEL.xlsx
+++ b/Retail Brands/LULU_MODEL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Models\Retail Brands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED56947-C5D3-4667-9DDD-2A1B685F8F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0393B81C-86DC-4C89-91F3-C1E7DAB22D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{74C982A1-EE30-4588-AA95-0E58E4E415F0}"/>
+    <workbookView xWindow="7140" yWindow="2280" windowWidth="28800" windowHeight="15345" activeTab="3" xr2:uid="{74C982A1-EE30-4588-AA95-0E58E4E415F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Alex:</t>
         </r>
@@ -96,7 +96,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -111,7 +111,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Alex:</t>
         </r>
@@ -120,7 +120,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Impairment of asset
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="119">
   <si>
     <t>Price</t>
   </si>
@@ -391,9 +391,6 @@
   </si>
   <si>
     <t>One of the least levered names in discretionary retail</t>
-  </si>
-  <si>
-    <t>Q52025</t>
   </si>
   <si>
     <t>Beginning</t>
@@ -502,13 +499,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -586,19 +589,6 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <i/>
@@ -719,81 +709,82 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -1133,7 +1124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB11C10-986F-41A4-B3DD-2A72A923BC11}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1178,7 +1169,7 @@
       <c r="B5" s="1">
         <v>121</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="49" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1318,28 +1309,28 @@
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="F2" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="G2" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="H2" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="I2" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="J2" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="K2" s="24" t="s">
         <v>109</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>110</v>
       </c>
       <c r="L2" s="24" t="s">
         <v>57</v>
@@ -3394,7 +3385,7 @@
     </row>
     <row r="27" spans="2:33" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AA27" s="6">
         <v>0.09</v>
@@ -3420,13 +3411,13 @@
     </row>
     <row r="28" spans="2:33" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Z28" s="6" t="s">
         <v>45</v>
       </c>
       <c r="AA28" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AB28" s="6">
         <v>0.11</v>
@@ -3449,7 +3440,7 @@
     </row>
     <row r="29" spans="2:33" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Z29" s="6" t="s">
         <v>45</v>
@@ -3478,7 +3469,7 @@
     </row>
     <row r="30" spans="2:33" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Z30" s="6" t="s">
         <v>45</v>
@@ -3507,7 +3498,7 @@
     </row>
     <row r="31" spans="2:33" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Z31" s="6" t="s">
         <v>45</v>
@@ -3536,7 +3527,7 @@
     </row>
     <row r="32" spans="2:33" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z32" s="6" t="s">
         <v>45</v>
@@ -3565,7 +3556,7 @@
     </row>
     <row r="33" spans="2:42" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z33" s="6" t="s">
         <v>45</v>
@@ -3594,7 +3585,7 @@
     </row>
     <row r="34" spans="2:42" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Z34" s="6" t="s">
         <v>45</v>
@@ -3658,10 +3649,10 @@
       <c r="AD36" s="12"/>
       <c r="AE36" s="12"/>
       <c r="AF36" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AG36" s="46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AH36" s="12"/>
       <c r="AI36" s="12"/>
@@ -3676,20 +3667,20 @@
     <row r="37" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B37" s="14"/>
       <c r="AF37" s="44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AG37" s="47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AP37" s="15"/>
     </row>
     <row r="38" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B38" s="14"/>
       <c r="AF38" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AG38" s="48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AP38" s="15"/>
     </row>
@@ -3725,10 +3716,10 @@
       <c r="AD39" s="18"/>
       <c r="AE39" s="18"/>
       <c r="AF39" s="45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AG39" s="42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AH39" s="18"/>
       <c r="AI39" s="18"/>
@@ -3837,7 +3828,7 @@
     <row r="46" spans="2:42" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B47" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C47" s="12"/>
       <c r="D47" s="12">
@@ -4019,433 +4010,433 @@
     </row>
     <row r="55" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="14"/>
-      <c r="C55" s="49"/>
-      <c r="D55" s="49"/>
-      <c r="E55" s="49"/>
-      <c r="F55" s="49"/>
-      <c r="G55" s="49"/>
-      <c r="H55" s="49"/>
-      <c r="I55" s="49"/>
-      <c r="J55" s="49"/>
-      <c r="K55" s="49"/>
-      <c r="L55" s="49"/>
-      <c r="M55" s="49"/>
-      <c r="N55" s="49"/>
-      <c r="O55" s="49"/>
-      <c r="P55" s="49"/>
-      <c r="Q55" s="49"/>
-      <c r="R55" s="49"/>
-      <c r="S55" s="49"/>
-      <c r="T55" s="49"/>
-      <c r="U55" s="49"/>
-      <c r="V55" s="49"/>
-      <c r="W55" s="49"/>
-      <c r="X55" s="49"/>
-      <c r="Y55" s="49"/>
-      <c r="Z55" s="49"/>
-      <c r="AA55" s="49"/>
-      <c r="AB55" s="49"/>
-      <c r="AC55" s="49"/>
-      <c r="AD55" s="49"/>
-      <c r="AE55" s="49"/>
-      <c r="AF55" s="49"/>
-      <c r="AG55" s="49"/>
-      <c r="AH55" s="49"/>
-      <c r="AI55" s="49"/>
-      <c r="AJ55" s="49"/>
-      <c r="AK55" s="49"/>
-      <c r="AL55" s="49"/>
-      <c r="AM55" s="49"/>
-      <c r="AN55" s="49"/>
-      <c r="AO55" s="49"/>
-      <c r="AP55" s="50"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="50"/>
+      <c r="H55" s="50"/>
+      <c r="I55" s="50"/>
+      <c r="J55" s="50"/>
+      <c r="K55" s="50"/>
+      <c r="L55" s="50"/>
+      <c r="M55" s="50"/>
+      <c r="N55" s="50"/>
+      <c r="O55" s="50"/>
+      <c r="P55" s="50"/>
+      <c r="Q55" s="50"/>
+      <c r="R55" s="50"/>
+      <c r="S55" s="50"/>
+      <c r="T55" s="50"/>
+      <c r="U55" s="50"/>
+      <c r="V55" s="50"/>
+      <c r="W55" s="50"/>
+      <c r="X55" s="50"/>
+      <c r="Y55" s="50"/>
+      <c r="Z55" s="50"/>
+      <c r="AA55" s="50"/>
+      <c r="AB55" s="50"/>
+      <c r="AC55" s="50"/>
+      <c r="AD55" s="50"/>
+      <c r="AE55" s="50"/>
+      <c r="AF55" s="50"/>
+      <c r="AG55" s="50"/>
+      <c r="AH55" s="50"/>
+      <c r="AI55" s="50"/>
+      <c r="AJ55" s="50"/>
+      <c r="AK55" s="50"/>
+      <c r="AL55" s="50"/>
+      <c r="AM55" s="50"/>
+      <c r="AN55" s="50"/>
+      <c r="AO55" s="50"/>
+      <c r="AP55" s="51"/>
     </row>
     <row r="56" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="14"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="49"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="49"/>
-      <c r="G56" s="49"/>
-      <c r="H56" s="49"/>
-      <c r="I56" s="49"/>
-      <c r="J56" s="49"/>
-      <c r="K56" s="49"/>
-      <c r="L56" s="49"/>
-      <c r="M56" s="49"/>
-      <c r="N56" s="49"/>
-      <c r="O56" s="49"/>
-      <c r="P56" s="49"/>
-      <c r="Q56" s="49"/>
-      <c r="R56" s="49"/>
-      <c r="S56" s="49"/>
-      <c r="T56" s="49"/>
-      <c r="U56" s="49"/>
-      <c r="V56" s="49"/>
-      <c r="W56" s="49"/>
-      <c r="X56" s="49"/>
-      <c r="Y56" s="49"/>
-      <c r="Z56" s="49"/>
-      <c r="AA56" s="49"/>
-      <c r="AB56" s="49"/>
-      <c r="AC56" s="49"/>
-      <c r="AD56" s="49"/>
-      <c r="AE56" s="49"/>
-      <c r="AF56" s="49"/>
-      <c r="AG56" s="49"/>
-      <c r="AH56" s="49"/>
-      <c r="AI56" s="49"/>
-      <c r="AJ56" s="49"/>
-      <c r="AK56" s="49"/>
-      <c r="AL56" s="49"/>
-      <c r="AM56" s="49"/>
-      <c r="AN56" s="49"/>
-      <c r="AO56" s="49"/>
-      <c r="AP56" s="50"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="50"/>
+      <c r="H56" s="50"/>
+      <c r="I56" s="50"/>
+      <c r="J56" s="50"/>
+      <c r="K56" s="50"/>
+      <c r="L56" s="50"/>
+      <c r="M56" s="50"/>
+      <c r="N56" s="50"/>
+      <c r="O56" s="50"/>
+      <c r="P56" s="50"/>
+      <c r="Q56" s="50"/>
+      <c r="R56" s="50"/>
+      <c r="S56" s="50"/>
+      <c r="T56" s="50"/>
+      <c r="U56" s="50"/>
+      <c r="V56" s="50"/>
+      <c r="W56" s="50"/>
+      <c r="X56" s="50"/>
+      <c r="Y56" s="50"/>
+      <c r="Z56" s="50"/>
+      <c r="AA56" s="50"/>
+      <c r="AB56" s="50"/>
+      <c r="AC56" s="50"/>
+      <c r="AD56" s="50"/>
+      <c r="AE56" s="50"/>
+      <c r="AF56" s="50"/>
+      <c r="AG56" s="50"/>
+      <c r="AH56" s="50"/>
+      <c r="AI56" s="50"/>
+      <c r="AJ56" s="50"/>
+      <c r="AK56" s="50"/>
+      <c r="AL56" s="50"/>
+      <c r="AM56" s="50"/>
+      <c r="AN56" s="50"/>
+      <c r="AO56" s="50"/>
+      <c r="AP56" s="51"/>
     </row>
     <row r="57" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="14"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="49"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="49"/>
-      <c r="G57" s="49"/>
-      <c r="H57" s="49"/>
-      <c r="I57" s="49"/>
-      <c r="J57" s="49"/>
-      <c r="K57" s="49"/>
-      <c r="L57" s="49"/>
-      <c r="M57" s="49"/>
-      <c r="N57" s="49"/>
-      <c r="O57" s="49"/>
-      <c r="P57" s="49"/>
-      <c r="Q57" s="49"/>
-      <c r="R57" s="49"/>
-      <c r="S57" s="49"/>
-      <c r="T57" s="49"/>
-      <c r="U57" s="49"/>
-      <c r="V57" s="49"/>
-      <c r="W57" s="49"/>
-      <c r="X57" s="49"/>
-      <c r="Y57" s="49"/>
-      <c r="Z57" s="49"/>
-      <c r="AA57" s="49"/>
-      <c r="AB57" s="49"/>
-      <c r="AC57" s="49"/>
-      <c r="AD57" s="49"/>
-      <c r="AE57" s="49"/>
-      <c r="AF57" s="49"/>
-      <c r="AG57" s="49"/>
-      <c r="AH57" s="49"/>
-      <c r="AI57" s="49"/>
-      <c r="AJ57" s="49"/>
-      <c r="AK57" s="49"/>
-      <c r="AL57" s="49"/>
-      <c r="AM57" s="49"/>
-      <c r="AN57" s="49"/>
-      <c r="AO57" s="49"/>
-      <c r="AP57" s="50"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="50"/>
+      <c r="G57" s="50"/>
+      <c r="H57" s="50"/>
+      <c r="I57" s="50"/>
+      <c r="J57" s="50"/>
+      <c r="K57" s="50"/>
+      <c r="L57" s="50"/>
+      <c r="M57" s="50"/>
+      <c r="N57" s="50"/>
+      <c r="O57" s="50"/>
+      <c r="P57" s="50"/>
+      <c r="Q57" s="50"/>
+      <c r="R57" s="50"/>
+      <c r="S57" s="50"/>
+      <c r="T57" s="50"/>
+      <c r="U57" s="50"/>
+      <c r="V57" s="50"/>
+      <c r="W57" s="50"/>
+      <c r="X57" s="50"/>
+      <c r="Y57" s="50"/>
+      <c r="Z57" s="50"/>
+      <c r="AA57" s="50"/>
+      <c r="AB57" s="50"/>
+      <c r="AC57" s="50"/>
+      <c r="AD57" s="50"/>
+      <c r="AE57" s="50"/>
+      <c r="AF57" s="50"/>
+      <c r="AG57" s="50"/>
+      <c r="AH57" s="50"/>
+      <c r="AI57" s="50"/>
+      <c r="AJ57" s="50"/>
+      <c r="AK57" s="50"/>
+      <c r="AL57" s="50"/>
+      <c r="AM57" s="50"/>
+      <c r="AN57" s="50"/>
+      <c r="AO57" s="50"/>
+      <c r="AP57" s="51"/>
     </row>
     <row r="58" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="14"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="49"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="49"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="49"/>
-      <c r="I58" s="49"/>
-      <c r="J58" s="49"/>
-      <c r="K58" s="49"/>
-      <c r="L58" s="49"/>
-      <c r="M58" s="49"/>
-      <c r="N58" s="49"/>
-      <c r="O58" s="49"/>
-      <c r="P58" s="49"/>
-      <c r="Q58" s="49"/>
-      <c r="R58" s="49"/>
-      <c r="S58" s="49"/>
-      <c r="T58" s="49"/>
-      <c r="U58" s="49"/>
-      <c r="V58" s="49"/>
-      <c r="W58" s="49"/>
-      <c r="X58" s="49"/>
-      <c r="Y58" s="49"/>
-      <c r="Z58" s="49"/>
-      <c r="AA58" s="49"/>
-      <c r="AB58" s="49"/>
-      <c r="AC58" s="49"/>
-      <c r="AD58" s="49"/>
-      <c r="AE58" s="49"/>
-      <c r="AF58" s="49"/>
-      <c r="AG58" s="49"/>
-      <c r="AH58" s="49"/>
-      <c r="AI58" s="49"/>
-      <c r="AJ58" s="49"/>
-      <c r="AK58" s="49"/>
-      <c r="AL58" s="49"/>
-      <c r="AM58" s="49"/>
-      <c r="AN58" s="49"/>
-      <c r="AO58" s="49"/>
-      <c r="AP58" s="50"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="50"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="50"/>
+      <c r="G58" s="50"/>
+      <c r="H58" s="50"/>
+      <c r="I58" s="50"/>
+      <c r="J58" s="50"/>
+      <c r="K58" s="50"/>
+      <c r="L58" s="50"/>
+      <c r="M58" s="50"/>
+      <c r="N58" s="50"/>
+      <c r="O58" s="50"/>
+      <c r="P58" s="50"/>
+      <c r="Q58" s="50"/>
+      <c r="R58" s="50"/>
+      <c r="S58" s="50"/>
+      <c r="T58" s="50"/>
+      <c r="U58" s="50"/>
+      <c r="V58" s="50"/>
+      <c r="W58" s="50"/>
+      <c r="X58" s="50"/>
+      <c r="Y58" s="50"/>
+      <c r="Z58" s="50"/>
+      <c r="AA58" s="50"/>
+      <c r="AB58" s="50"/>
+      <c r="AC58" s="50"/>
+      <c r="AD58" s="50"/>
+      <c r="AE58" s="50"/>
+      <c r="AF58" s="50"/>
+      <c r="AG58" s="50"/>
+      <c r="AH58" s="50"/>
+      <c r="AI58" s="50"/>
+      <c r="AJ58" s="50"/>
+      <c r="AK58" s="50"/>
+      <c r="AL58" s="50"/>
+      <c r="AM58" s="50"/>
+      <c r="AN58" s="50"/>
+      <c r="AO58" s="50"/>
+      <c r="AP58" s="51"/>
     </row>
     <row r="59" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="14"/>
-      <c r="C59" s="49"/>
-      <c r="D59" s="49"/>
-      <c r="E59" s="49"/>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="49"/>
-      <c r="I59" s="49"/>
-      <c r="J59" s="49"/>
-      <c r="K59" s="49"/>
-      <c r="L59" s="49"/>
-      <c r="M59" s="49"/>
-      <c r="N59" s="49"/>
-      <c r="O59" s="49"/>
-      <c r="P59" s="49"/>
-      <c r="Q59" s="49"/>
-      <c r="R59" s="49"/>
-      <c r="S59" s="49"/>
-      <c r="T59" s="49"/>
-      <c r="U59" s="49"/>
-      <c r="V59" s="49"/>
-      <c r="W59" s="49"/>
-      <c r="X59" s="49"/>
-      <c r="Y59" s="49"/>
-      <c r="Z59" s="49"/>
-      <c r="AA59" s="49"/>
-      <c r="AB59" s="49"/>
-      <c r="AC59" s="49"/>
-      <c r="AD59" s="49"/>
-      <c r="AE59" s="49"/>
-      <c r="AF59" s="49"/>
-      <c r="AG59" s="49"/>
-      <c r="AH59" s="49"/>
-      <c r="AI59" s="49"/>
-      <c r="AJ59" s="49"/>
-      <c r="AK59" s="49"/>
-      <c r="AL59" s="49"/>
-      <c r="AM59" s="49"/>
-      <c r="AN59" s="49"/>
-      <c r="AO59" s="49"/>
-      <c r="AP59" s="50"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="50"/>
+      <c r="H59" s="50"/>
+      <c r="I59" s="50"/>
+      <c r="J59" s="50"/>
+      <c r="K59" s="50"/>
+      <c r="L59" s="50"/>
+      <c r="M59" s="50"/>
+      <c r="N59" s="50"/>
+      <c r="O59" s="50"/>
+      <c r="P59" s="50"/>
+      <c r="Q59" s="50"/>
+      <c r="R59" s="50"/>
+      <c r="S59" s="50"/>
+      <c r="T59" s="50"/>
+      <c r="U59" s="50"/>
+      <c r="V59" s="50"/>
+      <c r="W59" s="50"/>
+      <c r="X59" s="50"/>
+      <c r="Y59" s="50"/>
+      <c r="Z59" s="50"/>
+      <c r="AA59" s="50"/>
+      <c r="AB59" s="50"/>
+      <c r="AC59" s="50"/>
+      <c r="AD59" s="50"/>
+      <c r="AE59" s="50"/>
+      <c r="AF59" s="50"/>
+      <c r="AG59" s="50"/>
+      <c r="AH59" s="50"/>
+      <c r="AI59" s="50"/>
+      <c r="AJ59" s="50"/>
+      <c r="AK59" s="50"/>
+      <c r="AL59" s="50"/>
+      <c r="AM59" s="50"/>
+      <c r="AN59" s="50"/>
+      <c r="AO59" s="50"/>
+      <c r="AP59" s="51"/>
     </row>
     <row r="60" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="14"/>
-      <c r="C60" s="49"/>
-      <c r="D60" s="49"/>
-      <c r="E60" s="49"/>
-      <c r="F60" s="49"/>
-      <c r="G60" s="49"/>
-      <c r="H60" s="49"/>
-      <c r="I60" s="49"/>
-      <c r="J60" s="49"/>
-      <c r="K60" s="49"/>
-      <c r="L60" s="49"/>
-      <c r="M60" s="49"/>
-      <c r="N60" s="49"/>
-      <c r="O60" s="49"/>
-      <c r="P60" s="49"/>
-      <c r="Q60" s="49"/>
-      <c r="R60" s="49"/>
-      <c r="S60" s="49"/>
-      <c r="T60" s="49"/>
-      <c r="U60" s="49"/>
-      <c r="V60" s="49"/>
-      <c r="W60" s="49"/>
-      <c r="X60" s="49"/>
-      <c r="Y60" s="49"/>
-      <c r="Z60" s="49"/>
-      <c r="AA60" s="49"/>
-      <c r="AB60" s="49"/>
-      <c r="AC60" s="49"/>
-      <c r="AD60" s="49"/>
-      <c r="AE60" s="49"/>
-      <c r="AF60" s="49"/>
-      <c r="AG60" s="49"/>
-      <c r="AH60" s="49"/>
-      <c r="AI60" s="49"/>
-      <c r="AJ60" s="49"/>
-      <c r="AK60" s="49"/>
-      <c r="AL60" s="49"/>
-      <c r="AM60" s="49"/>
-      <c r="AN60" s="49"/>
-      <c r="AO60" s="49"/>
-      <c r="AP60" s="50"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="50"/>
+      <c r="E60" s="50"/>
+      <c r="F60" s="50"/>
+      <c r="G60" s="50"/>
+      <c r="H60" s="50"/>
+      <c r="I60" s="50"/>
+      <c r="J60" s="50"/>
+      <c r="K60" s="50"/>
+      <c r="L60" s="50"/>
+      <c r="M60" s="50"/>
+      <c r="N60" s="50"/>
+      <c r="O60" s="50"/>
+      <c r="P60" s="50"/>
+      <c r="Q60" s="50"/>
+      <c r="R60" s="50"/>
+      <c r="S60" s="50"/>
+      <c r="T60" s="50"/>
+      <c r="U60" s="50"/>
+      <c r="V60" s="50"/>
+      <c r="W60" s="50"/>
+      <c r="X60" s="50"/>
+      <c r="Y60" s="50"/>
+      <c r="Z60" s="50"/>
+      <c r="AA60" s="50"/>
+      <c r="AB60" s="50"/>
+      <c r="AC60" s="50"/>
+      <c r="AD60" s="50"/>
+      <c r="AE60" s="50"/>
+      <c r="AF60" s="50"/>
+      <c r="AG60" s="50"/>
+      <c r="AH60" s="50"/>
+      <c r="AI60" s="50"/>
+      <c r="AJ60" s="50"/>
+      <c r="AK60" s="50"/>
+      <c r="AL60" s="50"/>
+      <c r="AM60" s="50"/>
+      <c r="AN60" s="50"/>
+      <c r="AO60" s="50"/>
+      <c r="AP60" s="51"/>
     </row>
     <row r="61" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="14"/>
-      <c r="C61" s="49"/>
-      <c r="D61" s="49"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="49"/>
-      <c r="G61" s="49"/>
-      <c r="H61" s="49"/>
-      <c r="I61" s="49"/>
-      <c r="J61" s="49"/>
-      <c r="K61" s="49"/>
-      <c r="L61" s="49"/>
-      <c r="M61" s="49"/>
-      <c r="N61" s="49"/>
-      <c r="O61" s="49"/>
-      <c r="P61" s="49"/>
-      <c r="Q61" s="49"/>
-      <c r="R61" s="49"/>
-      <c r="S61" s="49"/>
-      <c r="T61" s="49"/>
-      <c r="U61" s="49"/>
-      <c r="V61" s="49"/>
-      <c r="W61" s="49"/>
-      <c r="X61" s="49"/>
-      <c r="Y61" s="49"/>
-      <c r="Z61" s="49"/>
-      <c r="AA61" s="49"/>
-      <c r="AB61" s="49"/>
-      <c r="AC61" s="49"/>
-      <c r="AD61" s="49"/>
-      <c r="AE61" s="49"/>
-      <c r="AF61" s="49"/>
-      <c r="AG61" s="49"/>
-      <c r="AH61" s="49"/>
-      <c r="AI61" s="49"/>
-      <c r="AJ61" s="49"/>
-      <c r="AK61" s="49"/>
-      <c r="AL61" s="49"/>
-      <c r="AM61" s="49"/>
-      <c r="AN61" s="49"/>
-      <c r="AO61" s="49"/>
-      <c r="AP61" s="50"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="50"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="50"/>
+      <c r="H61" s="50"/>
+      <c r="I61" s="50"/>
+      <c r="J61" s="50"/>
+      <c r="K61" s="50"/>
+      <c r="L61" s="50"/>
+      <c r="M61" s="50"/>
+      <c r="N61" s="50"/>
+      <c r="O61" s="50"/>
+      <c r="P61" s="50"/>
+      <c r="Q61" s="50"/>
+      <c r="R61" s="50"/>
+      <c r="S61" s="50"/>
+      <c r="T61" s="50"/>
+      <c r="U61" s="50"/>
+      <c r="V61" s="50"/>
+      <c r="W61" s="50"/>
+      <c r="X61" s="50"/>
+      <c r="Y61" s="50"/>
+      <c r="Z61" s="50"/>
+      <c r="AA61" s="50"/>
+      <c r="AB61" s="50"/>
+      <c r="AC61" s="50"/>
+      <c r="AD61" s="50"/>
+      <c r="AE61" s="50"/>
+      <c r="AF61" s="50"/>
+      <c r="AG61" s="50"/>
+      <c r="AH61" s="50"/>
+      <c r="AI61" s="50"/>
+      <c r="AJ61" s="50"/>
+      <c r="AK61" s="50"/>
+      <c r="AL61" s="50"/>
+      <c r="AM61" s="50"/>
+      <c r="AN61" s="50"/>
+      <c r="AO61" s="50"/>
+      <c r="AP61" s="51"/>
     </row>
     <row r="62" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="14"/>
-      <c r="C62" s="49"/>
-      <c r="D62" s="49"/>
-      <c r="E62" s="49"/>
-      <c r="F62" s="49"/>
-      <c r="G62" s="49"/>
-      <c r="H62" s="49"/>
-      <c r="I62" s="49"/>
-      <c r="J62" s="49"/>
-      <c r="K62" s="49"/>
-      <c r="L62" s="49"/>
-      <c r="M62" s="49"/>
-      <c r="N62" s="49"/>
-      <c r="O62" s="49"/>
-      <c r="P62" s="49"/>
-      <c r="Q62" s="49"/>
-      <c r="R62" s="49"/>
-      <c r="S62" s="49"/>
-      <c r="T62" s="49"/>
-      <c r="U62" s="49"/>
-      <c r="V62" s="49"/>
-      <c r="W62" s="49"/>
-      <c r="X62" s="49"/>
-      <c r="Y62" s="49"/>
-      <c r="Z62" s="49"/>
-      <c r="AA62" s="49"/>
-      <c r="AB62" s="49"/>
-      <c r="AC62" s="49"/>
-      <c r="AD62" s="49"/>
-      <c r="AE62" s="49"/>
-      <c r="AF62" s="49"/>
-      <c r="AG62" s="49"/>
-      <c r="AH62" s="49"/>
-      <c r="AI62" s="49"/>
-      <c r="AJ62" s="49"/>
-      <c r="AK62" s="49"/>
-      <c r="AL62" s="49"/>
-      <c r="AM62" s="49"/>
-      <c r="AN62" s="49"/>
-      <c r="AO62" s="49"/>
-      <c r="AP62" s="50"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="50"/>
+      <c r="E62" s="50"/>
+      <c r="F62" s="50"/>
+      <c r="G62" s="50"/>
+      <c r="H62" s="50"/>
+      <c r="I62" s="50"/>
+      <c r="J62" s="50"/>
+      <c r="K62" s="50"/>
+      <c r="L62" s="50"/>
+      <c r="M62" s="50"/>
+      <c r="N62" s="50"/>
+      <c r="O62" s="50"/>
+      <c r="P62" s="50"/>
+      <c r="Q62" s="50"/>
+      <c r="R62" s="50"/>
+      <c r="S62" s="50"/>
+      <c r="T62" s="50"/>
+      <c r="U62" s="50"/>
+      <c r="V62" s="50"/>
+      <c r="W62" s="50"/>
+      <c r="X62" s="50"/>
+      <c r="Y62" s="50"/>
+      <c r="Z62" s="50"/>
+      <c r="AA62" s="50"/>
+      <c r="AB62" s="50"/>
+      <c r="AC62" s="50"/>
+      <c r="AD62" s="50"/>
+      <c r="AE62" s="50"/>
+      <c r="AF62" s="50"/>
+      <c r="AG62" s="50"/>
+      <c r="AH62" s="50"/>
+      <c r="AI62" s="50"/>
+      <c r="AJ62" s="50"/>
+      <c r="AK62" s="50"/>
+      <c r="AL62" s="50"/>
+      <c r="AM62" s="50"/>
+      <c r="AN62" s="50"/>
+      <c r="AO62" s="50"/>
+      <c r="AP62" s="51"/>
     </row>
     <row r="63" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="14"/>
-      <c r="C63" s="49"/>
-      <c r="D63" s="49"/>
-      <c r="E63" s="49"/>
-      <c r="F63" s="49"/>
-      <c r="G63" s="49"/>
-      <c r="H63" s="49"/>
-      <c r="I63" s="49"/>
-      <c r="J63" s="49"/>
-      <c r="K63" s="49"/>
-      <c r="L63" s="49"/>
-      <c r="M63" s="49"/>
-      <c r="N63" s="49"/>
-      <c r="O63" s="49"/>
-      <c r="P63" s="49"/>
-      <c r="Q63" s="49"/>
-      <c r="R63" s="49"/>
-      <c r="S63" s="49"/>
-      <c r="T63" s="49"/>
-      <c r="U63" s="49"/>
-      <c r="V63" s="49"/>
-      <c r="W63" s="49"/>
-      <c r="X63" s="49"/>
-      <c r="Y63" s="49"/>
-      <c r="Z63" s="49"/>
-      <c r="AA63" s="49"/>
-      <c r="AB63" s="49"/>
-      <c r="AC63" s="49"/>
-      <c r="AD63" s="49"/>
-      <c r="AE63" s="49"/>
-      <c r="AF63" s="49"/>
-      <c r="AG63" s="49"/>
-      <c r="AH63" s="49"/>
-      <c r="AI63" s="49"/>
-      <c r="AJ63" s="49"/>
-      <c r="AK63" s="49"/>
-      <c r="AL63" s="49"/>
-      <c r="AM63" s="49"/>
-      <c r="AN63" s="49"/>
-      <c r="AO63" s="49"/>
-      <c r="AP63" s="50"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="50"/>
+      <c r="F63" s="50"/>
+      <c r="G63" s="50"/>
+      <c r="H63" s="50"/>
+      <c r="I63" s="50"/>
+      <c r="J63" s="50"/>
+      <c r="K63" s="50"/>
+      <c r="L63" s="50"/>
+      <c r="M63" s="50"/>
+      <c r="N63" s="50"/>
+      <c r="O63" s="50"/>
+      <c r="P63" s="50"/>
+      <c r="Q63" s="50"/>
+      <c r="R63" s="50"/>
+      <c r="S63" s="50"/>
+      <c r="T63" s="50"/>
+      <c r="U63" s="50"/>
+      <c r="V63" s="50"/>
+      <c r="W63" s="50"/>
+      <c r="X63" s="50"/>
+      <c r="Y63" s="50"/>
+      <c r="Z63" s="50"/>
+      <c r="AA63" s="50"/>
+      <c r="AB63" s="50"/>
+      <c r="AC63" s="50"/>
+      <c r="AD63" s="50"/>
+      <c r="AE63" s="50"/>
+      <c r="AF63" s="50"/>
+      <c r="AG63" s="50"/>
+      <c r="AH63" s="50"/>
+      <c r="AI63" s="50"/>
+      <c r="AJ63" s="50"/>
+      <c r="AK63" s="50"/>
+      <c r="AL63" s="50"/>
+      <c r="AM63" s="50"/>
+      <c r="AN63" s="50"/>
+      <c r="AO63" s="50"/>
+      <c r="AP63" s="51"/>
     </row>
     <row r="64" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="14"/>
-      <c r="C64" s="49"/>
-      <c r="D64" s="49"/>
-      <c r="E64" s="49"/>
-      <c r="F64" s="49"/>
-      <c r="G64" s="49"/>
-      <c r="H64" s="49"/>
-      <c r="I64" s="49"/>
-      <c r="J64" s="49"/>
-      <c r="K64" s="49"/>
-      <c r="L64" s="49"/>
-      <c r="M64" s="49"/>
-      <c r="N64" s="49"/>
-      <c r="O64" s="49"/>
-      <c r="P64" s="49"/>
-      <c r="Q64" s="49"/>
-      <c r="R64" s="49"/>
-      <c r="S64" s="49"/>
-      <c r="T64" s="49"/>
-      <c r="U64" s="49"/>
-      <c r="V64" s="49"/>
-      <c r="W64" s="49"/>
-      <c r="X64" s="49"/>
-      <c r="Y64" s="49"/>
-      <c r="Z64" s="49"/>
-      <c r="AA64" s="49"/>
-      <c r="AB64" s="49"/>
-      <c r="AC64" s="49"/>
-      <c r="AD64" s="49"/>
-      <c r="AE64" s="49"/>
-      <c r="AF64" s="49"/>
-      <c r="AG64" s="49"/>
-      <c r="AH64" s="49"/>
-      <c r="AI64" s="49"/>
-      <c r="AJ64" s="49"/>
-      <c r="AK64" s="49"/>
-      <c r="AL64" s="49"/>
-      <c r="AM64" s="49"/>
-      <c r="AN64" s="49"/>
-      <c r="AO64" s="49"/>
-      <c r="AP64" s="50"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="50"/>
+      <c r="G64" s="50"/>
+      <c r="H64" s="50"/>
+      <c r="I64" s="50"/>
+      <c r="J64" s="50"/>
+      <c r="K64" s="50"/>
+      <c r="L64" s="50"/>
+      <c r="M64" s="50"/>
+      <c r="N64" s="50"/>
+      <c r="O64" s="50"/>
+      <c r="P64" s="50"/>
+      <c r="Q64" s="50"/>
+      <c r="R64" s="50"/>
+      <c r="S64" s="50"/>
+      <c r="T64" s="50"/>
+      <c r="U64" s="50"/>
+      <c r="V64" s="50"/>
+      <c r="W64" s="50"/>
+      <c r="X64" s="50"/>
+      <c r="Y64" s="50"/>
+      <c r="Z64" s="50"/>
+      <c r="AA64" s="50"/>
+      <c r="AB64" s="50"/>
+      <c r="AC64" s="50"/>
+      <c r="AD64" s="50"/>
+      <c r="AE64" s="50"/>
+      <c r="AF64" s="50"/>
+      <c r="AG64" s="50"/>
+      <c r="AH64" s="50"/>
+      <c r="AI64" s="50"/>
+      <c r="AJ64" s="50"/>
+      <c r="AK64" s="50"/>
+      <c r="AL64" s="50"/>
+      <c r="AM64" s="50"/>
+      <c r="AN64" s="50"/>
+      <c r="AO64" s="50"/>
+      <c r="AP64" s="51"/>
     </row>
     <row r="65" spans="2:42" ht="15" x14ac:dyDescent="0.25">
       <c r="B65" s="14"/>
@@ -4630,8 +4621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D091CCF-214C-4799-9BEE-D3FB22B6975A}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4646,16 +4637,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -4713,8 +4704,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>86</v>
+      <c r="A5" s="52" t="s">
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>767</v>
@@ -5004,7 +4995,7 @@
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" s="32">
         <v>6.96</v>
@@ -5033,7 +5024,7 @@
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B10" s="32">
         <v>2.11</v>
@@ -5062,7 +5053,7 @@
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" s="32">
         <v>24.71</v>
@@ -5149,15 +5140,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C341BEE4C9A91F44BB4A4EF8E0A71E02" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db93f7cdcc50be3ddb7642c8d50e9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="878aac0c-df32-40a9-a231-d93e9c7b9b1a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b63aaf3684aa43c37ed0cc1f5c2cf36e" ns3:_="">
     <xsd:import namespace="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
@@ -5301,6 +5283,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5308,14 +5299,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9D266F6-4EBB-4FCE-8CE5-50B9641EB015}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5329,6 +5312,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>